<commit_message>
Add 2-opt per route & show distance per route
</commit_message>
<xml_diff>
--- a/solution.xlsx
+++ b/solution.xlsx
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10">
@@ -546,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -557,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>115</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12">
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>118</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
@@ -579,7 +579,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14">
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15">
@@ -601,7 +601,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16">
@@ -612,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17">
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18">
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -645,7 +645,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20">
@@ -656,7 +656,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21">
@@ -667,7 +667,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22">
@@ -678,7 +678,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>103</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23">
@@ -689,7 +689,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>77</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24">
@@ -700,7 +700,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>74</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25">
@@ -711,7 +711,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>82</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
@@ -722,7 +722,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>71</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27">
@@ -733,7 +733,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
@@ -931,7 +931,7 @@
         <v>17</v>
       </c>
       <c r="C45" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46">
@@ -953,7 +953,7 @@
         <v>19</v>
       </c>
       <c r="C47" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48">
@@ -1129,7 +1129,7 @@
         <v>35</v>
       </c>
       <c r="C63" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64">
@@ -1140,7 +1140,7 @@
         <v>36</v>
       </c>
       <c r="C64" t="n">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65">
@@ -1283,7 +1283,7 @@
         <v>6</v>
       </c>
       <c r="C77" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78">
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="C78" t="n">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79">
@@ -1305,7 +1305,7 @@
         <v>8</v>
       </c>
       <c r="C79" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80">
@@ -1316,7 +1316,7 @@
         <v>9</v>
       </c>
       <c r="C80" t="n">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81">
@@ -1327,7 +1327,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82">
@@ -1338,7 +1338,7 @@
         <v>11</v>
       </c>
       <c r="C82" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83">
@@ -1349,7 +1349,7 @@
         <v>12</v>
       </c>
       <c r="C83" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84">
@@ -1360,7 +1360,7 @@
         <v>13</v>
       </c>
       <c r="C84" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85">
@@ -1371,7 +1371,7 @@
         <v>14</v>
       </c>
       <c r="C85" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86">
@@ -1382,7 +1382,7 @@
         <v>15</v>
       </c>
       <c r="C86" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87">
@@ -1393,7 +1393,7 @@
         <v>16</v>
       </c>
       <c r="C87" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88">
@@ -1404,7 +1404,7 @@
         <v>17</v>
       </c>
       <c r="C88" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89">
@@ -1415,7 +1415,7 @@
         <v>18</v>
       </c>
       <c r="C89" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90">
@@ -1426,7 +1426,7 @@
         <v>19</v>
       </c>
       <c r="C90" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91">
@@ -1437,7 +1437,7 @@
         <v>20</v>
       </c>
       <c r="C91" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="92">
@@ -1448,7 +1448,7 @@
         <v>21</v>
       </c>
       <c r="C92" t="n">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93">
@@ -1459,7 +1459,7 @@
         <v>22</v>
       </c>
       <c r="C93" t="n">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94">
@@ -1470,7 +1470,7 @@
         <v>23</v>
       </c>
       <c r="C94" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95">
@@ -1481,7 +1481,7 @@
         <v>24</v>
       </c>
       <c r="C95" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96">
@@ -1492,7 +1492,7 @@
         <v>25</v>
       </c>
       <c r="C96" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="97">
@@ -1503,7 +1503,7 @@
         <v>26</v>
       </c>
       <c r="C97" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="98">
@@ -1514,7 +1514,7 @@
         <v>27</v>
       </c>
       <c r="C98" t="n">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="99">
@@ -1525,7 +1525,7 @@
         <v>28</v>
       </c>
       <c r="C99" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100">
@@ -1536,7 +1536,7 @@
         <v>29</v>
       </c>
       <c r="C100" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101">
@@ -1547,7 +1547,7 @@
         <v>30</v>
       </c>
       <c r="C101" t="n">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102">
@@ -1558,7 +1558,7 @@
         <v>31</v>
       </c>
       <c r="C102" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103">
@@ -1569,7 +1569,7 @@
         <v>32</v>
       </c>
       <c r="C103" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104">
@@ -1580,7 +1580,7 @@
         <v>33</v>
       </c>
       <c r="C104" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105">
@@ -1591,7 +1591,7 @@
         <v>34</v>
       </c>
       <c r="C105" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106">
@@ -1602,7 +1602,7 @@
         <v>35</v>
       </c>
       <c r="C106" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107">
@@ -1613,7 +1613,7 @@
         <v>36</v>
       </c>
       <c r="C107" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108">
@@ -1701,7 +1701,7 @@
         <v>7</v>
       </c>
       <c r="C115" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="116">
@@ -1712,7 +1712,7 @@
         <v>8</v>
       </c>
       <c r="C116" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="117">
@@ -1723,7 +1723,7 @@
         <v>9</v>
       </c>
       <c r="C117" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="118">

</xml_diff>

<commit_message>
Code with simulated annealing added
</commit_message>
<xml_diff>
--- a/solution.xlsx
+++ b/solution.xlsx
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -546,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -557,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -579,7 +579,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
@@ -601,7 +601,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
@@ -612,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
@@ -656,7 +656,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21">
@@ -667,7 +667,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22">
@@ -678,7 +678,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
@@ -689,7 +689,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -700,7 +700,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
@@ -711,7 +711,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26">
@@ -722,7 +722,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -744,7 +744,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29">
@@ -755,7 +755,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
@@ -766,7 +766,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31">
@@ -777,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
@@ -788,7 +788,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
@@ -799,7 +799,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -810,7 +810,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -821,7 +821,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
@@ -1426,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="C90" t="n">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91">
@@ -1437,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="C91" t="n">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92">
@@ -1448,7 +1448,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="n">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93">
@@ -1459,7 +1459,7 @@
         <v>5</v>
       </c>
       <c r="C93" t="n">
-        <v>68</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94">
@@ -1470,7 +1470,7 @@
         <v>6</v>
       </c>
       <c r="C94" t="n">
-        <v>58</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95">
@@ -1481,7 +1481,7 @@
         <v>7</v>
       </c>
       <c r="C95" t="n">
-        <v>59</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96">
@@ -1492,7 +1492,7 @@
         <v>8</v>
       </c>
       <c r="C96" t="n">
-        <v>57</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97">
@@ -1503,7 +1503,7 @@
         <v>9</v>
       </c>
       <c r="C97" t="n">
-        <v>62</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98">
@@ -1514,7 +1514,7 @@
         <v>10</v>
       </c>
       <c r="C98" t="n">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99">
@@ -1525,7 +1525,7 @@
         <v>11</v>
       </c>
       <c r="C99" t="n">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="100">
@@ -1536,7 +1536,7 @@
         <v>12</v>
       </c>
       <c r="C100" t="n">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101">
@@ -1547,7 +1547,7 @@
         <v>13</v>
       </c>
       <c r="C101" t="n">
-        <v>56</v>
+        <v>112</v>
       </c>
     </row>
     <row r="102">
@@ -1558,7 +1558,7 @@
         <v>14</v>
       </c>
       <c r="C102" t="n">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103">
@@ -1569,7 +1569,7 @@
         <v>15</v>
       </c>
       <c r="C103" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104">
@@ -1580,7 +1580,7 @@
         <v>16</v>
       </c>
       <c r="C104" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105">
@@ -1591,7 +1591,7 @@
         <v>17</v>
       </c>
       <c r="C105" t="n">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106">
@@ -1602,7 +1602,7 @@
         <v>18</v>
       </c>
       <c r="C106" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="107">
@@ -1613,7 +1613,7 @@
         <v>19</v>
       </c>
       <c r="C107" t="n">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="108">
@@ -1624,7 +1624,7 @@
         <v>20</v>
       </c>
       <c r="C108" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="109">
@@ -1635,7 +1635,7 @@
         <v>21</v>
       </c>
       <c r="C109" t="n">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="110">
@@ -1646,7 +1646,7 @@
         <v>22</v>
       </c>
       <c r="C110" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="111">
@@ -1657,7 +1657,7 @@
         <v>23</v>
       </c>
       <c r="C111" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="112">
@@ -1668,7 +1668,7 @@
         <v>24</v>
       </c>
       <c r="C112" t="n">
-        <v>87</v>
+        <v>58</v>
       </c>
     </row>
     <row r="113">
@@ -1679,7 +1679,7 @@
         <v>25</v>
       </c>
       <c r="C113" t="n">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="114">
@@ -1690,7 +1690,7 @@
         <v>26</v>
       </c>
       <c r="C114" t="n">
-        <v>95</v>
+        <v>57</v>
       </c>
     </row>
     <row r="115">
@@ -1701,7 +1701,7 @@
         <v>27</v>
       </c>
       <c r="C115" t="n">
-        <v>101</v>
+        <v>62</v>
       </c>
     </row>
     <row r="116">
@@ -1712,7 +1712,7 @@
         <v>28</v>
       </c>
       <c r="C116" t="n">
-        <v>102</v>
+        <v>76</v>
       </c>
     </row>
     <row r="117">
@@ -1723,7 +1723,7 @@
         <v>29</v>
       </c>
       <c r="C117" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="118">
@@ -1734,7 +1734,7 @@
         <v>30</v>
       </c>
       <c r="C118" t="n">
-        <v>98</v>
+        <v>63</v>
       </c>
     </row>
     <row r="119">
@@ -1745,7 +1745,7 @@
         <v>31</v>
       </c>
       <c r="C119" t="n">
-        <v>93</v>
+        <v>64</v>
       </c>
     </row>
     <row r="120">
@@ -1756,7 +1756,7 @@
         <v>32</v>
       </c>
       <c r="C120" t="n">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="121">
@@ -1767,7 +1767,7 @@
         <v>33</v>
       </c>
       <c r="C121" t="n">
-        <v>112</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Runn full pipeline for each given split point and find the best route
</commit_message>
<xml_diff>
--- a/solution.xlsx
+++ b/solution.xlsx
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -546,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -557,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -579,7 +579,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
@@ -601,7 +601,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
@@ -612,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
@@ -656,7 +656,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21">
@@ -667,7 +667,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22">
@@ -678,7 +678,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
@@ -689,7 +689,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -700,7 +700,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
@@ -711,7 +711,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26">
@@ -722,7 +722,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -744,7 +744,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29">
@@ -755,7 +755,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
@@ -766,7 +766,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31">
@@ -777,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
@@ -788,7 +788,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
@@ -799,7 +799,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -810,7 +810,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -821,7 +821,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
@@ -1426,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="C90" t="n">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91">
@@ -1437,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="C91" t="n">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92">
@@ -1448,7 +1448,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="n">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93">
@@ -1459,7 +1459,7 @@
         <v>5</v>
       </c>
       <c r="C93" t="n">
-        <v>68</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94">
@@ -1470,7 +1470,7 @@
         <v>6</v>
       </c>
       <c r="C94" t="n">
-        <v>58</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95">
@@ -1481,7 +1481,7 @@
         <v>7</v>
       </c>
       <c r="C95" t="n">
-        <v>59</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96">
@@ -1492,7 +1492,7 @@
         <v>8</v>
       </c>
       <c r="C96" t="n">
-        <v>57</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97">
@@ -1503,7 +1503,7 @@
         <v>9</v>
       </c>
       <c r="C97" t="n">
-        <v>62</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98">
@@ -1514,7 +1514,7 @@
         <v>10</v>
       </c>
       <c r="C98" t="n">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99">
@@ -1525,7 +1525,7 @@
         <v>11</v>
       </c>
       <c r="C99" t="n">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="100">
@@ -1536,7 +1536,7 @@
         <v>12</v>
       </c>
       <c r="C100" t="n">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101">
@@ -1547,7 +1547,7 @@
         <v>13</v>
       </c>
       <c r="C101" t="n">
-        <v>56</v>
+        <v>112</v>
       </c>
     </row>
     <row r="102">
@@ -1558,7 +1558,7 @@
         <v>14</v>
       </c>
       <c r="C102" t="n">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103">
@@ -1569,7 +1569,7 @@
         <v>15</v>
       </c>
       <c r="C103" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104">
@@ -1580,7 +1580,7 @@
         <v>16</v>
       </c>
       <c r="C104" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105">
@@ -1591,7 +1591,7 @@
         <v>17</v>
       </c>
       <c r="C105" t="n">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106">
@@ -1602,7 +1602,7 @@
         <v>18</v>
       </c>
       <c r="C106" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="107">
@@ -1613,7 +1613,7 @@
         <v>19</v>
       </c>
       <c r="C107" t="n">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="108">
@@ -1624,7 +1624,7 @@
         <v>20</v>
       </c>
       <c r="C108" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="109">
@@ -1635,7 +1635,7 @@
         <v>21</v>
       </c>
       <c r="C109" t="n">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="110">
@@ -1646,7 +1646,7 @@
         <v>22</v>
       </c>
       <c r="C110" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="111">
@@ -1657,7 +1657,7 @@
         <v>23</v>
       </c>
       <c r="C111" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="112">
@@ -1668,7 +1668,7 @@
         <v>24</v>
       </c>
       <c r="C112" t="n">
-        <v>87</v>
+        <v>58</v>
       </c>
     </row>
     <row r="113">
@@ -1679,7 +1679,7 @@
         <v>25</v>
       </c>
       <c r="C113" t="n">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="114">
@@ -1690,7 +1690,7 @@
         <v>26</v>
       </c>
       <c r="C114" t="n">
-        <v>95</v>
+        <v>57</v>
       </c>
     </row>
     <row r="115">
@@ -1701,7 +1701,7 @@
         <v>27</v>
       </c>
       <c r="C115" t="n">
-        <v>101</v>
+        <v>62</v>
       </c>
     </row>
     <row r="116">
@@ -1712,7 +1712,7 @@
         <v>28</v>
       </c>
       <c r="C116" t="n">
-        <v>102</v>
+        <v>76</v>
       </c>
     </row>
     <row r="117">
@@ -1723,7 +1723,7 @@
         <v>29</v>
       </c>
       <c r="C117" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="118">
@@ -1734,7 +1734,7 @@
         <v>30</v>
       </c>
       <c r="C118" t="n">
-        <v>98</v>
+        <v>63</v>
       </c>
     </row>
     <row r="119">
@@ -1745,7 +1745,7 @@
         <v>31</v>
       </c>
       <c r="C119" t="n">
-        <v>93</v>
+        <v>64</v>
       </c>
     </row>
     <row r="120">
@@ -1756,7 +1756,7 @@
         <v>32</v>
       </c>
       <c r="C120" t="n">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="121">
@@ -1767,7 +1767,7 @@
         <v>33</v>
       </c>
       <c r="C121" t="n">
-        <v>112</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>